<commit_message>
change chain task data type
</commit_message>
<xml_diff>
--- a/config/config_test.xlsx
+++ b/config/config_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b60e98ec5e6769d/デスクトップ/mapd/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{9C7E034B-BB54-4B31-9E71-829C94C03384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA0D8126-D8E3-4ABC-9CE2-21EBDA948FD9}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{9C7E034B-BB54-4B31-9E71-829C94C03384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84571184-2747-42A5-BE8F-C4DD4F38DCCB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-16780" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agents" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="22">
   <si>
     <t>.</t>
     <phoneticPr fontId="1"/>
@@ -206,6 +206,10 @@
 </file>
 
 <file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -547,7 +551,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -585,8 +589,8 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
+      <c r="C2">
+        <v>-1</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -640,16 +644,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -936,9 +940,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1151,27 +1158,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE09FB56-7470-43BD-92C5-92AC7F73F832}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8C77A44-1FB2-4E19-93B8-F60FE118FD4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0027cc79-339f-4d1a-8619-966c060bb560"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="363ad6d6-8e13-4d1a-b321-414a9449fc18"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1196,9 +1191,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8C77A44-1FB2-4E19-93B8-F60FE118FD4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE09FB56-7470-43BD-92C5-92AC7F73F832}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="0027cc79-339f-4d1a-8619-966c060bb560"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="363ad6d6-8e13-4d1a-b321-414a9449fc18"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>